<commit_message>
time on shift and calculation fixed
</commit_message>
<xml_diff>
--- a/app/static/excel/employee_data1.xlsx
+++ b/app/static/excel/employee_data1.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyDesktop\Projects\KKL-Attendance-System\app\static\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\my Project\KKL-Attendance-System\app\static\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3BF82D4-28EF-4673-ACE5-0C52FDC25B17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{490CF897-654F-4186-9D8F-C42DDCD52B6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet_1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" iterateDelta="1E-4"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -1989,8 +1989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N103" sqref="N103"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="E97" sqref="E97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>